<commit_message>
Remove GST from DToPaSoVAbIC
</commit_message>
<xml_diff>
--- a/InputData/io-model/DToPaSoVAbIC/Domestic Taxes on Prod as Shr of Val Added by ISIC Code.xlsx
+++ b/InputData/io-model/DToPaSoVAbIC/Domestic Taxes on Prod as Shr of Val Added by ISIC Code.xlsx
@@ -1,30 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\io-model\DToPaSoVAbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39529954-3602-4AD0-968E-E6259D93B7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA2AFE0-EA8E-4BD3-9BD9-AC9167D8EE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BVAbIC" sheetId="21" r:id="rId2"/>
     <sheet name="KLEMS VA" sheetId="22" r:id="rId3"/>
     <sheet name="Corporate Taxes" sheetId="23" r:id="rId4"/>
-    <sheet name="Approximate GST Rates" sheetId="26" r:id="rId5"/>
-    <sheet name="GST" sheetId="25" r:id="rId6"/>
-    <sheet name="DToPaSoVAbIC" sheetId="2" r:id="rId7"/>
+    <sheet name="DToPaSoVAbIC" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="CAP_CT" localSheetId="4">#REF!</definedName>
     <definedName name="CAP_CT">#REF!</definedName>
-    <definedName name="CAP_GFCF" localSheetId="4">#REF!</definedName>
     <definedName name="CAP_GFCF">#REF!</definedName>
     <definedName name="CAP_IT">#REF!</definedName>
     <definedName name="CAP_OCon">#REF!</definedName>
@@ -63,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="255">
   <si>
     <t>Source:</t>
   </si>
@@ -563,144 +559,6 @@
     <t>each of those components to the ISIC codes used in the EPS.</t>
   </si>
   <si>
-    <t>D01T03: Agriculture, forestry and fishing</t>
-  </si>
-  <si>
-    <t>D05: Coal mining</t>
-  </si>
-  <si>
-    <t>D06: Oil and gas extraction</t>
-  </si>
-  <si>
-    <t>D07T08: Mining and quarrying of uranium and non-energy-producing products</t>
-  </si>
-  <si>
-    <t>D09: Mining support service activities</t>
-  </si>
-  <si>
-    <t>D10T12: Food products, beverages and tobacco</t>
-  </si>
-  <si>
-    <t>D13T15: Textiles, wearing apparel, leather and related products</t>
-  </si>
-  <si>
-    <t>D16: Wood and products of wood and cork</t>
-  </si>
-  <si>
-    <t>D17T18: Paper products and printing</t>
-  </si>
-  <si>
-    <t>D19: Coke and refined petroleum products</t>
-  </si>
-  <si>
-    <t>D20: Chemicals</t>
-  </si>
-  <si>
-    <t>D21: Pharmaceuticals</t>
-  </si>
-  <si>
-    <t>D22: Rubber and plastic products</t>
-  </si>
-  <si>
-    <t>D239: Cement and other nometallic minerals</t>
-  </si>
-  <si>
-    <t>D24: Metals</t>
-  </si>
-  <si>
-    <t>D25: Fabricated metal products</t>
-  </si>
-  <si>
-    <t>D26: Computer, electronic and optical products</t>
-  </si>
-  <si>
-    <t>D27: Electrical equipment</t>
-  </si>
-  <si>
-    <t>D28: Machinery and equipment, nec</t>
-  </si>
-  <si>
-    <t>D29: Motor vehicles, trailers and semi-trailers</t>
-  </si>
-  <si>
-    <t>D30: Other transport equipment</t>
-  </si>
-  <si>
-    <t>D31T33: Other manufacturing; repair and installation of machinery and equipment</t>
-  </si>
-  <si>
-    <t>D351: Electricity generation and distribution, energy pipelines and gas processing, and water and wate</t>
-  </si>
-  <si>
-    <t>D41T43: Construction</t>
-  </si>
-  <si>
-    <t>D45T47: Wholesale and retail trade; repair of motor vehicles</t>
-  </si>
-  <si>
-    <t>D49T53: Transportation and storage</t>
-  </si>
-  <si>
-    <t>D55T56: Accomodation and food services</t>
-  </si>
-  <si>
-    <t>D58T60: Publishing, audiovisual and broadcasting activities</t>
-  </si>
-  <si>
-    <t>D61: Telecommunications</t>
-  </si>
-  <si>
-    <t>D62T63: IT and other information services</t>
-  </si>
-  <si>
-    <t>D64T66: Financial and insurance activities</t>
-  </si>
-  <si>
-    <t>D68: Real estate activities</t>
-  </si>
-  <si>
-    <t>D69T82: Other business sector services</t>
-  </si>
-  <si>
-    <t>D84: Public admin. and defence; compulsory social security</t>
-  </si>
-  <si>
-    <t>D85: Education</t>
-  </si>
-  <si>
-    <t>D86T88: Human health and social work</t>
-  </si>
-  <si>
-    <t>D90T96: Arts, entertainment, recreation and other service activities</t>
-  </si>
-  <si>
-    <t>D97T98: Private households with employed persons</t>
-  </si>
-  <si>
-    <t>Tax Rate</t>
-  </si>
-  <si>
-    <t>Total GST Revenue (2018-2019)</t>
-  </si>
-  <si>
-    <t>Approximate Tax Rates Applied to KLEMS Value Add Figures (2018-2019)</t>
-  </si>
-  <si>
-    <t>Tax Collected</t>
-  </si>
-  <si>
-    <t>Total Tax Collected Using Approximate Tax Rates</t>
-  </si>
-  <si>
-    <t>Ratio of Actual GST Revenue to Revenue with Approximate Tax Rates</t>
-  </si>
-  <si>
-    <t>GST Tax Rates Adjusted to Match Total Collected 2018-2019 Revenue</t>
-  </si>
-  <si>
-    <t>*average of 5% and 12% rates</t>
-  </si>
-  <si>
     <t>Approximate Tax Rates</t>
   </si>
   <si>
@@ -962,19 +820,10 @@
     <t>We compile industry specific tax rates using reported total corporate tax collection as a share of value add, mapping</t>
   </si>
   <si>
-    <t>by estimating the average tax rate paid by ISIC code based on applicable GST rates by product and the types</t>
-  </si>
-  <si>
-    <t>of products or services contained within each ISIC code, then scaling those rates so that we produce the</t>
-  </si>
-  <si>
-    <t>correct GST revenue for the 2018-2019 FY.</t>
-  </si>
-  <si>
-    <t>We then approximate the tax rates paid by each industry</t>
-  </si>
-  <si>
-    <t>The reported tax rates are the sum of corporate and GST taxes.</t>
+    <t>We do not capture India's GST in this file, meaning that the policy-induced changes in GST revenue will</t>
+  </si>
+  <si>
+    <t>be excluded from the India EPS.</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1013,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1209,12 +1058,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1503,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1598,12 +1442,12 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>213</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1613,12 +1457,12 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
-        <v>214</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1641,7 +1485,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>298</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1649,29 +1493,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>302</v>
-      </c>
-    </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>299</v>
+      <c r="A32" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>303</v>
+      <c r="A33" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -6484,7 +6313,7 @@
         <f>$B$40/SUM(I2,Q2,S2,W2,T2)</f>
         <v>0.12340408240956703</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="30">
         <f t="shared" si="1"/>
         <v>2.3384963217858205E-2</v>
       </c>
@@ -6623,1048 +6452,902 @@
       <c r="J8"/>
     </row>
     <row r="9" spans="1:39" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
-        <v>216</v>
-      </c>
-      <c r="B9" s="31">
+      <c r="A9" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9">
         <v>319.41000000000003</v>
       </c>
-      <c r="C9" s="31"/>
       <c r="D9" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="31"/>
       <c r="J9"/>
     </row>
     <row r="10" spans="1:39" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="s">
-        <v>217</v>
-      </c>
-      <c r="B10" s="31">
+      <c r="A10" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10">
         <v>343.64</v>
       </c>
-      <c r="C10" s="31"/>
       <c r="D10" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="31"/>
       <c r="J10"/>
     </row>
     <row r="11" spans="1:39" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="B11" s="31">
+      <c r="A11" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11">
         <v>183.95</v>
       </c>
-      <c r="C11" s="31"/>
       <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="31"/>
       <c r="J11"/>
     </row>
     <row r="12" spans="1:39" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="B12" s="31">
+      <c r="A12" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12">
         <v>442.67</v>
       </c>
-      <c r="C12" s="31"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="31"/>
       <c r="J12"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A13" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="31">
+      <c r="A13" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13">
         <v>16.59</v>
       </c>
-      <c r="C13" s="31"/>
       <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="31"/>
       <c r="J13"/>
     </row>
     <row r="14" spans="1:39" ht="58" x14ac:dyDescent="0.35">
-      <c r="A14" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="B14" s="31">
+      <c r="A14" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14">
         <v>5.18</v>
       </c>
-      <c r="C14" s="31"/>
       <c r="D14" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="31"/>
       <c r="J14"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A15" s="33" t="s">
-        <v>295</v>
-      </c>
-      <c r="B15" s="31">
+      <c r="A15" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B15">
         <v>61.3</v>
       </c>
-      <c r="C15" s="31"/>
       <c r="D15" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="31"/>
       <c r="J15"/>
     </row>
     <row r="16" spans="1:39" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="B16" s="31">
+      <c r="A16" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16">
         <v>13369.23</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31" t="s">
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="31"/>
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="B17" s="31">
+      <c r="A17" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
         <v>9292.34</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31" t="s">
+      <c r="D17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="31"/>
       <c r="J17"/>
     </row>
     <row r="18" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="B18" s="31">
+      <c r="A18" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18">
         <v>2360.77</v>
       </c>
-      <c r="C18" s="31"/>
       <c r="D18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="31"/>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="31">
+      <c r="A19" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19">
         <v>2060.15</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31" t="s">
+      <c r="D19" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="31"/>
       <c r="J19"/>
     </row>
     <row r="20" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="B20" s="31">
+      <c r="A20" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B20">
         <v>2576.94</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31" t="s">
+      <c r="D20" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="31"/>
       <c r="J20"/>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
-        <v>225</v>
-      </c>
-      <c r="B21" s="31">
+      <c r="A21" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B21">
         <v>21568.27</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31" t="s">
+      <c r="D21" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="31"/>
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="33" t="s">
-        <v>226</v>
-      </c>
-      <c r="B22" s="31">
+      <c r="A22" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22">
         <v>16249.56</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31" t="s">
+      <c r="D22" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="31"/>
       <c r="J22"/>
     </row>
     <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="33" t="s">
-        <v>227</v>
-      </c>
-      <c r="B23" s="31">
+      <c r="A23" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23">
         <v>12021.07</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31" t="s">
+      <c r="D23" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="31"/>
       <c r="J23"/>
     </row>
     <row r="24" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="B24" s="31">
+      <c r="A24" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B24">
         <v>9723.18</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="31" t="s">
         <v>18</v>
       </c>
       <c r="J24"/>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="B25" s="31">
+      <c r="A25" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B25">
         <v>11521.97</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31" t="s">
+      <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="E25" s="31"/>
       <c r="J25"/>
     </row>
     <row r="26" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="B26" s="31">
+      <c r="A26" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26">
         <v>7941.02</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31" t="s">
+      <c r="D26" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="31"/>
       <c r="J26"/>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="B27" s="31">
+      <c r="A27" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27">
         <v>6143.59</v>
       </c>
-      <c r="C27" s="31"/>
       <c r="D27" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="31"/>
       <c r="J27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="B28" s="31">
+      <c r="A28" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28">
         <v>4279.62</v>
       </c>
-      <c r="C28" s="31"/>
       <c r="D28" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="31"/>
       <c r="J28"/>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="33" t="s">
-        <v>233</v>
-      </c>
-      <c r="B29" s="31">
+      <c r="A29" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29">
         <v>3793.39</v>
       </c>
-      <c r="C29" s="31"/>
       <c r="D29" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="31"/>
       <c r="J29"/>
     </row>
     <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="33" t="s">
-        <v>234</v>
-      </c>
-      <c r="B30" s="31">
+      <c r="A30" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30">
         <v>3506.82</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31" t="s">
+      <c r="D30" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="31"/>
       <c r="J30"/>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="B31" s="31">
+      <c r="A31" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31">
         <v>3337.25</v>
       </c>
-      <c r="C31" s="31"/>
       <c r="D31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="31"/>
       <c r="J31"/>
     </row>
     <row r="32" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="B32" s="31">
+      <c r="A32" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32">
         <v>1706.14</v>
       </c>
-      <c r="C32" s="31"/>
       <c r="D32" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="31"/>
       <c r="J32"/>
     </row>
     <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="33" t="s">
-        <v>237</v>
-      </c>
-      <c r="B33" s="31">
+      <c r="A33" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33">
         <v>484.53</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31" t="s">
+      <c r="D33" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="31"/>
       <c r="J33"/>
     </row>
     <row r="34" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="33" t="s">
-        <v>238</v>
-      </c>
-      <c r="B34" s="31">
+      <c r="A34" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34">
         <v>1958.45</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31" t="s">
+      <c r="D34" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="31"/>
       <c r="J34"/>
     </row>
     <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="B35" s="31">
+      <c r="A35" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35">
         <v>2063.5</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31" t="s">
+      <c r="D35" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="31"/>
       <c r="J35"/>
     </row>
     <row r="36" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="33" t="s">
-        <v>240</v>
-      </c>
-      <c r="B36" s="31">
+      <c r="A36" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B36">
         <v>1788.93</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31" t="s">
+      <c r="D36" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="31"/>
       <c r="J36"/>
     </row>
     <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="33" t="s">
-        <v>241</v>
-      </c>
-      <c r="B37" s="31">
+      <c r="A37" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37">
         <v>1294.6099999999999</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31" t="s">
+      <c r="D37" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
       <c r="J37"/>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="B38" s="31">
+      <c r="A38" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38">
         <v>1700.9</v>
       </c>
-      <c r="C38" s="31"/>
       <c r="D38" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="31"/>
       <c r="J38"/>
     </row>
     <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="B39" s="31">
+      <c r="A39" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39">
         <v>1528.58</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="31" t="s">
         <v>18</v>
       </c>
       <c r="J39"/>
     </row>
     <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="33" t="s">
-        <v>297</v>
-      </c>
-      <c r="B40" s="31">
+      <c r="A40" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B40">
         <v>71797.47</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="31"/>
+      <c r="D40" s="31"/>
       <c r="J40"/>
     </row>
     <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="B41" s="31">
+      <c r="A41" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41">
         <v>10370.07</v>
       </c>
-      <c r="C41" s="31"/>
       <c r="D41" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="31"/>
       <c r="J41"/>
     </row>
     <row r="42" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="33" t="s">
-        <v>245</v>
-      </c>
-      <c r="B42" s="31">
+      <c r="A42" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42">
         <v>2999.79</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31" t="s">
+      <c r="D42" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="31"/>
       <c r="J42"/>
     </row>
     <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="B43" s="31">
+      <c r="A43" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B43">
         <v>15.37</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31" t="s">
+      <c r="D43" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="31"/>
       <c r="J43"/>
     </row>
     <row r="44" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="33" t="s">
-        <v>247</v>
-      </c>
-      <c r="B44" s="31">
+      <c r="A44" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B44">
         <v>157.58000000000001</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31" t="s">
+      <c r="D44" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="31"/>
       <c r="J44"/>
     </row>
     <row r="45" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A45" s="33" t="s">
-        <v>248</v>
-      </c>
-      <c r="B45" s="31">
+      <c r="A45" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B45">
         <v>6614.91</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31" t="s">
+      <c r="D45" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="31"/>
       <c r="J45"/>
     </row>
     <row r="46" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="B46" s="31">
+      <c r="A46" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46">
         <v>3515.92</v>
       </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31" t="s">
+      <c r="D46" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="31"/>
       <c r="J46"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="B47" s="31">
+      <c r="A47" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47">
         <v>6742.47</v>
       </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31" t="s">
+      <c r="D47" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="31"/>
       <c r="J47"/>
     </row>
     <row r="48" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="B48" s="31">
+      <c r="A48" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B48">
         <v>1464.42</v>
       </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31" t="s">
+      <c r="D48" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="31"/>
       <c r="J48"/>
     </row>
     <row r="49" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A49" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="B49" s="31">
+      <c r="A49" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B49">
         <v>1359.58</v>
       </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31" t="s">
+      <c r="D49" t="s">
         <v>29</v>
       </c>
-      <c r="E49" s="31"/>
       <c r="J49"/>
     </row>
     <row r="50" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="B50" s="31">
+      <c r="A50" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50">
         <v>550.49</v>
       </c>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31" t="s">
+      <c r="D50" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="31"/>
       <c r="J50"/>
     </row>
     <row r="51" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="B51" s="31">
+      <c r="A51" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51">
         <v>401.63</v>
       </c>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31" t="s">
+      <c r="D51" t="s">
         <v>29</v>
       </c>
-      <c r="E51" s="31"/>
       <c r="J51"/>
     </row>
     <row r="52" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A52" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="B52" s="31">
+      <c r="A52" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B52">
         <v>2906.04</v>
       </c>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31" t="s">
+      <c r="D52" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="31"/>
       <c r="J52"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A53" s="33" t="s">
-        <v>256</v>
-      </c>
-      <c r="B53" s="31">
+      <c r="A53" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53">
         <v>289.60000000000002</v>
       </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31" t="s">
+      <c r="D53" t="s">
         <v>30</v>
       </c>
-      <c r="E53" s="31"/>
       <c r="J53"/>
     </row>
     <row r="54" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="33" t="s">
-        <v>257</v>
-      </c>
-      <c r="B54" s="31">
+      <c r="A54" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B54">
         <v>3285.67</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31" t="s">
+      <c r="D54" t="s">
         <v>22</v>
       </c>
-      <c r="E54" s="31"/>
       <c r="J54"/>
     </row>
     <row r="55" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="B55" s="31">
+      <c r="A55" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="B55">
         <v>1003.2</v>
       </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31" t="s">
+      <c r="D55" t="s">
         <v>22</v>
       </c>
-      <c r="E55" s="31"/>
       <c r="J55"/>
     </row>
     <row r="56" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="B56" s="31">
+      <c r="A56" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B56">
         <v>1175.3499999999999</v>
       </c>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31" t="s">
+      <c r="D56" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="31"/>
       <c r="J56"/>
     </row>
     <row r="57" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A57" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="B57" s="31">
+      <c r="A57" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B57">
         <v>759.47</v>
       </c>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31" t="s">
+      <c r="D57" t="s">
         <v>22</v>
       </c>
-      <c r="E57" s="31"/>
       <c r="J57"/>
     </row>
     <row r="58" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="B58" s="31">
+      <c r="A58" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B58">
         <v>623.25</v>
       </c>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31" t="s">
+      <c r="D58" t="s">
         <v>22</v>
       </c>
-      <c r="E58" s="31"/>
       <c r="J58"/>
     </row>
     <row r="59" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="B59" s="31">
+      <c r="A59" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B59">
         <v>18478.240000000002</v>
       </c>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31" t="s">
+      <c r="D59" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="31"/>
       <c r="J59"/>
     </row>
     <row r="60" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="B60" s="31">
+      <c r="A60" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B60">
         <v>1924.99</v>
       </c>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31" t="s">
+      <c r="D60" t="s">
         <v>24</v>
       </c>
-      <c r="E60" s="31"/>
       <c r="J60"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A61" s="33" t="s">
-        <v>264</v>
-      </c>
-      <c r="B61" s="31">
+      <c r="A61" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B61">
         <v>193.61</v>
       </c>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31" t="s">
+      <c r="D61" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="31"/>
       <c r="J61"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A62" s="33" t="s">
-        <v>265</v>
-      </c>
-      <c r="B62" s="31">
+      <c r="A62" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B62">
         <v>816.79</v>
       </c>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31" t="s">
+      <c r="D62" t="s">
         <v>23</v>
       </c>
-      <c r="E62" s="31"/>
       <c r="J62"/>
     </row>
     <row r="63" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="33" t="s">
-        <v>266</v>
-      </c>
-      <c r="B63" s="31">
+      <c r="A63" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B63">
         <v>4351.59</v>
       </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31" t="s">
+      <c r="D63" t="s">
         <v>23</v>
       </c>
-      <c r="E63" s="31"/>
       <c r="J63"/>
     </row>
     <row r="64" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="33" t="s">
-        <v>267</v>
-      </c>
-      <c r="B64" s="31">
+      <c r="A64" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B64">
         <v>6207.68</v>
       </c>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31" t="s">
+      <c r="D64" t="s">
         <v>26</v>
       </c>
-      <c r="E64" s="31"/>
       <c r="J64"/>
     </row>
     <row r="65" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="33" t="s">
-        <v>268</v>
-      </c>
-      <c r="B65" s="31">
+      <c r="A65" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B65">
         <v>38773.71</v>
       </c>
-      <c r="C65" s="31"/>
-      <c r="D65" s="31" t="s">
+      <c r="D65" t="s">
         <v>28</v>
       </c>
-      <c r="E65" s="31"/>
       <c r="J65"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A66" s="33" t="s">
-        <v>269</v>
-      </c>
-      <c r="B66" s="31">
+      <c r="A66" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B66">
         <v>9469.0499999999993</v>
       </c>
-      <c r="C66" s="31"/>
-      <c r="D66" s="31" t="s">
+      <c r="D66" t="s">
         <v>28</v>
       </c>
-      <c r="E66" s="31"/>
       <c r="J66"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A67" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="B67" s="31">
+      <c r="A67" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B67">
         <v>7026.33</v>
       </c>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31" t="s">
+      <c r="D67" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="31"/>
       <c r="J67"/>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="B68" s="31">
+      <c r="A68" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B68">
         <v>50317.74</v>
       </c>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31" t="s">
+      <c r="D68" t="s">
         <v>28</v>
       </c>
-      <c r="E68" s="31"/>
       <c r="J68"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A69" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="B69" s="31">
+      <c r="A69" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69">
         <v>37416.19</v>
       </c>
-      <c r="C69" s="31"/>
-      <c r="D69" s="31" t="s">
+      <c r="D69" t="s">
         <v>27</v>
       </c>
-      <c r="E69" s="31"/>
       <c r="J69"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A70" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="B70" s="31">
+      <c r="A70" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B70">
         <v>15381.53</v>
       </c>
-      <c r="C70" s="31"/>
-      <c r="D70" s="31" t="s">
+      <c r="D70" t="s">
         <v>27</v>
       </c>
-      <c r="E70" s="31"/>
       <c r="J70"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A71" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="B71" s="31">
+      <c r="A71" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B71">
         <v>2005.41</v>
       </c>
-      <c r="C71" s="31"/>
-      <c r="D71" s="31" t="s">
+      <c r="D71" t="s">
         <v>30</v>
       </c>
-      <c r="E71" s="31"/>
       <c r="J71"/>
     </row>
     <row r="72" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="B72" s="31">
+      <c r="A72" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B72">
         <v>1654.95</v>
       </c>
-      <c r="C72" s="31"/>
-      <c r="D72" s="31" t="s">
+      <c r="D72" t="s">
         <v>27</v>
       </c>
-      <c r="E72" s="31"/>
       <c r="J72"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="B73" s="31">
+      <c r="A73" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B73">
         <v>352.3</v>
       </c>
-      <c r="C73" s="31"/>
-      <c r="D73" s="31" t="s">
+      <c r="D73" t="s">
         <v>30</v>
       </c>
-      <c r="E73" s="31"/>
       <c r="J73"/>
     </row>
     <row r="74" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A74" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="B74" s="31">
+      <c r="A74" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B74">
         <v>1751.49</v>
       </c>
-      <c r="C74" s="31"/>
-      <c r="D74" s="31" t="s">
+      <c r="D74" t="s">
         <v>30</v>
       </c>
-      <c r="E74" s="31"/>
       <c r="J74"/>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="B75" s="31">
+      <c r="A75" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B75">
         <v>82.87</v>
       </c>
-      <c r="C75" s="31"/>
-      <c r="D75" s="31" t="s">
+      <c r="D75" t="s">
         <v>30</v>
       </c>
-      <c r="E75" s="31"/>
       <c r="J75"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="B76" s="31">
+      <c r="A76" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B76">
         <v>518.72</v>
       </c>
-      <c r="C76" s="31"/>
-      <c r="D76" s="31" t="s">
+      <c r="D76" t="s">
         <v>30</v>
       </c>
-      <c r="E76" s="31"/>
       <c r="J76"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="B77" s="31">
+      <c r="A77" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B77">
         <v>63.79</v>
       </c>
-      <c r="C77" s="31"/>
-      <c r="D77" s="31" t="s">
+      <c r="D77" t="s">
         <v>30</v>
       </c>
-      <c r="E77" s="31"/>
       <c r="J77"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="B78" s="31">
+      <c r="A78" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B78">
         <v>1292.93</v>
       </c>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31" t="s">
+      <c r="D78" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="31"/>
       <c r="J78"/>
     </row>
     <row r="79" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="33" t="s">
-        <v>282</v>
-      </c>
-      <c r="B79" s="31">
+      <c r="A79" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="B79">
         <v>208.3</v>
       </c>
-      <c r="C79" s="31"/>
-      <c r="D79" s="31" t="s">
+      <c r="D79" t="s">
         <v>32</v>
       </c>
-      <c r="E79" s="31"/>
       <c r="J79"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A80" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="B80" s="31">
+      <c r="A80" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80">
         <v>61.54</v>
       </c>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31" t="s">
+      <c r="D80" t="s">
         <v>32</v>
       </c>
-      <c r="E80" s="31"/>
       <c r="J80"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A81" s="33" t="s">
-        <v>284</v>
-      </c>
-      <c r="B81" s="31">
+      <c r="A81" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B81">
         <v>506.7</v>
       </c>
-      <c r="C81" s="31"/>
-      <c r="D81" s="31" t="s">
+      <c r="D81" t="s">
         <v>32</v>
       </c>
-      <c r="E81" s="31"/>
       <c r="J81"/>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A82" s="33" t="s">
-        <v>285</v>
-      </c>
-      <c r="B82" s="31">
+      <c r="A82" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82">
         <v>907.83</v>
       </c>
-      <c r="C82" s="31"/>
       <c r="D82" t="s">
         <v>33</v>
       </c>
-      <c r="E82" s="31"/>
       <c r="J82"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A83" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="B83" s="31">
+      <c r="A83" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B83">
         <v>407.18</v>
       </c>
       <c r="D83" t="s">
@@ -7673,10 +7356,10 @@
       <c r="J83"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A84" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="B84" s="31">
+      <c r="A84" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="B84">
         <v>386.39</v>
       </c>
       <c r="D84" t="s">
@@ -7685,10 +7368,10 @@
       <c r="J84"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A85" s="33" t="s">
-        <v>288</v>
-      </c>
-      <c r="B85" s="31">
+      <c r="A85" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B85">
         <v>211.57</v>
       </c>
       <c r="D85" t="s">
@@ -7697,10 +7380,10 @@
       <c r="J85"/>
     </row>
     <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A86" s="33" t="s">
-        <v>289</v>
-      </c>
-      <c r="B86" s="31">
+      <c r="A86" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="B86">
         <v>352.93</v>
       </c>
       <c r="D86" t="s">
@@ -7709,10 +7392,10 @@
       <c r="J86"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A87" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="B87" s="31">
+      <c r="A87" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B87">
         <v>31.06</v>
       </c>
       <c r="D87" t="s">
@@ -7721,10 +7404,10 @@
       <c r="J87"/>
     </row>
     <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A88" s="33" t="s">
-        <v>291</v>
-      </c>
-      <c r="B88" s="31">
+      <c r="A88" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="B88">
         <v>2286.67</v>
       </c>
       <c r="D88" t="s">
@@ -7733,10 +7416,10 @@
       <c r="J88"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A89" s="33" t="s">
-        <v>292</v>
-      </c>
-      <c r="B89" s="31">
+      <c r="A89" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B89">
         <v>345.05</v>
       </c>
       <c r="D89" t="s">
@@ -7745,10 +7428,10 @@
       <c r="J89"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A90" s="33" t="s">
-        <v>293</v>
-      </c>
-      <c r="B90" s="31">
+      <c r="A90" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B90">
         <v>1010.13</v>
       </c>
       <c r="D90" t="s">
@@ -7757,10 +7440,10 @@
       <c r="J90"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A91" s="33" t="s">
+      <c r="A91" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B91" s="31">
+      <c r="B91">
         <v>29709.46</v>
       </c>
       <c r="D91" t="s">
@@ -7775,1220 +7458,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBF2198-ACE7-443B-806D-39BB8F4197D4}">
-  <dimension ref="A1:AQ4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AI3" sqref="AI3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:43" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43" s="3" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="P2" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="AB2" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="AD2" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="AE2" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="AF2" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="AG2" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="AH2" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="AI2" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="AJ2" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="AK2" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="AL2" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="AM2" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="G3" s="9">
-        <f>AVERAGE(0.05,0.12)</f>
-        <v>8.4999999999999992E-2</v>
-      </c>
-      <c r="H3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="I3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="J3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="K3" s="9">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="N3" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="P3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="Q3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="R3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="S3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="T3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="U3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="V3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="W3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="X3" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="Z3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="AA3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="AB3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="AC3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="AD3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="AE3" s="9">
-        <v>0.12</v>
-      </c>
-      <c r="AF3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="AG3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="AH3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="AI3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="9">
-        <v>0.18</v>
-      </c>
-      <c r="AM3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="G4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EB9AFD-4B07-436F-AB69-CEECFB40FA55}">
-  <dimension ref="A1:AM13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:39" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="30">
-        <v>581559.30000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="B4" t="str">
-        <f>'KLEMS VA'!AP32</f>
-        <v>ISIC 01T03</v>
-      </c>
-      <c r="C4" t="str">
-        <f>'KLEMS VA'!AQ32</f>
-        <v>ISIC 05</v>
-      </c>
-      <c r="D4" t="str">
-        <f>'KLEMS VA'!AR32</f>
-        <v>ISIC 06</v>
-      </c>
-      <c r="E4" t="str">
-        <f>'KLEMS VA'!AS32</f>
-        <v>ISIC 07T08</v>
-      </c>
-      <c r="F4" t="str">
-        <f>'KLEMS VA'!AT32</f>
-        <v>ISIC 09</v>
-      </c>
-      <c r="G4" t="str">
-        <f>'KLEMS VA'!AU32</f>
-        <v>ISIC 10T12</v>
-      </c>
-      <c r="H4" t="str">
-        <f>'KLEMS VA'!AV32</f>
-        <v>ISIC 13T15</v>
-      </c>
-      <c r="I4" t="str">
-        <f>'KLEMS VA'!AW32</f>
-        <v>ISIC 16</v>
-      </c>
-      <c r="J4" t="str">
-        <f>'KLEMS VA'!AX32</f>
-        <v>ISIC 17T18</v>
-      </c>
-      <c r="K4" t="str">
-        <f>'KLEMS VA'!AY32</f>
-        <v>ISIC 19</v>
-      </c>
-      <c r="L4" t="str">
-        <f>'KLEMS VA'!AZ32</f>
-        <v>ISIC 20</v>
-      </c>
-      <c r="M4" t="str">
-        <f>'KLEMS VA'!BA32</f>
-        <v>ISIC 21</v>
-      </c>
-      <c r="N4" t="str">
-        <f>'KLEMS VA'!BB32</f>
-        <v>ISIC 22</v>
-      </c>
-      <c r="O4" t="str">
-        <f>'KLEMS VA'!BC32</f>
-        <v>ISIC 23</v>
-      </c>
-      <c r="P4" t="str">
-        <f>'KLEMS VA'!BD32</f>
-        <v>ISIC 24</v>
-      </c>
-      <c r="Q4" t="str">
-        <f>'KLEMS VA'!BE32</f>
-        <v>ISIC 25</v>
-      </c>
-      <c r="R4" t="str">
-        <f>'KLEMS VA'!BF32</f>
-        <v>ISIC 26</v>
-      </c>
-      <c r="S4" t="str">
-        <f>'KLEMS VA'!BG32</f>
-        <v>ISIC 27</v>
-      </c>
-      <c r="T4" t="str">
-        <f>'KLEMS VA'!BH32</f>
-        <v>ISIC 28</v>
-      </c>
-      <c r="U4" t="str">
-        <f>'KLEMS VA'!BI32</f>
-        <v>ISIC 29</v>
-      </c>
-      <c r="V4" t="str">
-        <f>'KLEMS VA'!BJ32</f>
-        <v>ISIC 30</v>
-      </c>
-      <c r="W4" t="str">
-        <f>'KLEMS VA'!BK32</f>
-        <v>ISIC 31T33</v>
-      </c>
-      <c r="X4" t="str">
-        <f>'KLEMS VA'!BL32</f>
-        <v>ISIC 35T39</v>
-      </c>
-      <c r="Y4" t="str">
-        <f>'KLEMS VA'!BM32</f>
-        <v>ISIC 41T43</v>
-      </c>
-      <c r="Z4" t="str">
-        <f>'KLEMS VA'!BN32</f>
-        <v>ISIC 45T47</v>
-      </c>
-      <c r="AA4" t="str">
-        <f>'KLEMS VA'!BO32</f>
-        <v>ISIC 49T53</v>
-      </c>
-      <c r="AB4" t="str">
-        <f>'KLEMS VA'!BP32</f>
-        <v>ISIC 55T56</v>
-      </c>
-      <c r="AC4" t="str">
-        <f>'KLEMS VA'!BQ32</f>
-        <v>ISIC 58T60</v>
-      </c>
-      <c r="AD4" t="str">
-        <f>'KLEMS VA'!BR32</f>
-        <v>ISIC 61</v>
-      </c>
-      <c r="AE4" t="str">
-        <f>'KLEMS VA'!BS32</f>
-        <v>ISIC 62T63</v>
-      </c>
-      <c r="AF4" t="str">
-        <f>'KLEMS VA'!BT32</f>
-        <v>ISIC 64T66</v>
-      </c>
-      <c r="AG4" t="str">
-        <f>'KLEMS VA'!BU32</f>
-        <v>ISIC 68</v>
-      </c>
-      <c r="AH4" t="str">
-        <f>'KLEMS VA'!BV32</f>
-        <v>ISIC 69T82</v>
-      </c>
-      <c r="AI4" t="str">
-        <f>'KLEMS VA'!BW32</f>
-        <v>ISIC 84</v>
-      </c>
-      <c r="AJ4" t="str">
-        <f>'KLEMS VA'!BX32</f>
-        <v>ISIC 85</v>
-      </c>
-      <c r="AK4" t="str">
-        <f>'KLEMS VA'!BY32</f>
-        <v>ISIC 86T88</v>
-      </c>
-      <c r="AL4" t="str">
-        <f>'KLEMS VA'!BZ32</f>
-        <v>ISIC 90T96</v>
-      </c>
-      <c r="AM4" t="str">
-        <f>'KLEMS VA'!CA32</f>
-        <v>ISIC 97T98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5">
-        <f>'KLEMS VA'!AP33*'Approximate GST Rates'!B3</f>
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f>'KLEMS VA'!AQ33*'Approximate GST Rates'!C3</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f>'KLEMS VA'!AR33*'Approximate GST Rates'!D3</f>
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>'KLEMS VA'!AS33*'Approximate GST Rates'!E3</f>
-        <v>2191.5258969652205</v>
-      </c>
-      <c r="F5">
-        <f>'KLEMS VA'!AT33*'Approximate GST Rates'!F3</f>
-        <v>7361.3273574559671</v>
-      </c>
-      <c r="G5">
-        <f>'KLEMS VA'!AU33*'Approximate GST Rates'!G3</f>
-        <v>28108.217877444844</v>
-      </c>
-      <c r="H5">
-        <f>'KLEMS VA'!AV33*'Approximate GST Rates'!H3</f>
-        <v>43301.69138274304</v>
-      </c>
-      <c r="I5">
-        <f>'KLEMS VA'!AW33*'Approximate GST Rates'!I3</f>
-        <v>5604.7840894499359</v>
-      </c>
-      <c r="J5">
-        <f>'KLEMS VA'!AX33*'Approximate GST Rates'!J3</f>
-        <v>8728.1728048274417</v>
-      </c>
-      <c r="K5">
-        <f>'KLEMS VA'!AY33*'Approximate GST Rates'!K3</f>
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f>'KLEMS VA'!AZ33*'Approximate GST Rates'!L3</f>
-        <v>46091.995044479532</v>
-      </c>
-      <c r="M5">
-        <f>'KLEMS VA'!BA33*'Approximate GST Rates'!M3</f>
-        <v>7930.1920221897853</v>
-      </c>
-      <c r="N5">
-        <f>'KLEMS VA'!BB33*'Approximate GST Rates'!N3</f>
-        <v>5167.5766236746022</v>
-      </c>
-      <c r="O5">
-        <f>'KLEMS VA'!BC33*'Approximate GST Rates'!O3</f>
-        <v>21448.773452876452</v>
-      </c>
-      <c r="P5">
-        <f>'KLEMS VA'!BD33*'Approximate GST Rates'!P3</f>
-        <v>26048.928490773436</v>
-      </c>
-      <c r="Q5">
-        <f>'KLEMS VA'!BE33*'Approximate GST Rates'!Q3</f>
-        <v>26661.03209174595</v>
-      </c>
-      <c r="R5">
-        <f>'KLEMS VA'!BF33*'Approximate GST Rates'!R3</f>
-        <v>9333.849313498109</v>
-      </c>
-      <c r="S5">
-        <f>'KLEMS VA'!BG33*'Approximate GST Rates'!S3</f>
-        <v>11858.310530396178</v>
-      </c>
-      <c r="T5">
-        <f>'KLEMS VA'!BH33*'Approximate GST Rates'!T3</f>
-        <v>23600.189200227109</v>
-      </c>
-      <c r="U5">
-        <f>'KLEMS VA'!BI33*'Approximate GST Rates'!U3</f>
-        <v>40763.997676810526</v>
-      </c>
-      <c r="V5">
-        <f>'KLEMS VA'!BJ33*'Approximate GST Rates'!V3</f>
-        <v>20294.207960760374</v>
-      </c>
-      <c r="W5">
-        <f>'KLEMS VA'!BK33*'Approximate GST Rates'!W3</f>
-        <v>10979.642748344339</v>
-      </c>
-      <c r="X5">
-        <f>'KLEMS VA'!BL33*'Approximate GST Rates'!X3</f>
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <f>'KLEMS VA'!BM33*'Approximate GST Rates'!Y3</f>
-        <v>161975.44021971259</v>
-      </c>
-      <c r="Z5">
-        <f>'KLEMS VA'!BN33*'Approximate GST Rates'!Z3</f>
-        <v>234515.77536656265</v>
-      </c>
-      <c r="AA5">
-        <f>'KLEMS VA'!BO33*'Approximate GST Rates'!AA3</f>
-        <v>96869.419306389813</v>
-      </c>
-      <c r="AB5">
-        <f>'KLEMS VA'!BP33*'Approximate GST Rates'!AB3</f>
-        <v>21682.743072998714</v>
-      </c>
-      <c r="AC5">
-        <f>'KLEMS VA'!BQ33*'Approximate GST Rates'!AC3</f>
-        <v>10469.407212936308</v>
-      </c>
-      <c r="AD5">
-        <f>'KLEMS VA'!BR33*'Approximate GST Rates'!AD3</f>
-        <v>35980.025505901409</v>
-      </c>
-      <c r="AE5">
-        <f>'KLEMS VA'!BS33*'Approximate GST Rates'!AE3</f>
-        <v>55645.171334384329</v>
-      </c>
-      <c r="AF5">
-        <f>'KLEMS VA'!BT33*'Approximate GST Rates'!AF3</f>
-        <v>171961.88607575113</v>
-      </c>
-      <c r="AG5">
-        <f>'KLEMS VA'!BU33*'Approximate GST Rates'!AG3</f>
-        <v>150317.5326980954</v>
-      </c>
-      <c r="AH5">
-        <f>'KLEMS VA'!BV33*'Approximate GST Rates'!AH3</f>
-        <v>251494.74553845965</v>
-      </c>
-      <c r="AI5">
-        <f>'KLEMS VA'!BW33*'Approximate GST Rates'!AI3</f>
-        <v>0</v>
-      </c>
-      <c r="AJ5">
-        <f>'KLEMS VA'!BX33*'Approximate GST Rates'!AJ3</f>
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <f>'KLEMS VA'!BY33*'Approximate GST Rates'!AK3</f>
-        <v>0</v>
-      </c>
-      <c r="AL5">
-        <f>'KLEMS VA'!BZ33*'Approximate GST Rates'!AL3</f>
-        <v>38888.211748207104</v>
-      </c>
-      <c r="AM5">
-        <f>'KLEMS VA'!CA33*'Approximate GST Rates'!AM3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B7" s="30">
-        <f>SUM(B5:AM5)</f>
-        <v>1575274.7726440621</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B8">
-        <f>B1/B7</f>
-        <v>0.36917959336317324</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="B11" t="str">
-        <f>'KLEMS VA'!AP32</f>
-        <v>ISIC 01T03</v>
-      </c>
-      <c r="C11" t="str">
-        <f>'KLEMS VA'!AQ32</f>
-        <v>ISIC 05</v>
-      </c>
-      <c r="D11" t="str">
-        <f>'KLEMS VA'!AR32</f>
-        <v>ISIC 06</v>
-      </c>
-      <c r="E11" t="str">
-        <f>'KLEMS VA'!AS32</f>
-        <v>ISIC 07T08</v>
-      </c>
-      <c r="F11" t="str">
-        <f>'KLEMS VA'!AT32</f>
-        <v>ISIC 09</v>
-      </c>
-      <c r="G11" t="str">
-        <f>'KLEMS VA'!AU32</f>
-        <v>ISIC 10T12</v>
-      </c>
-      <c r="H11" t="str">
-        <f>'KLEMS VA'!AV32</f>
-        <v>ISIC 13T15</v>
-      </c>
-      <c r="I11" t="str">
-        <f>'KLEMS VA'!AW32</f>
-        <v>ISIC 16</v>
-      </c>
-      <c r="J11" t="str">
-        <f>'KLEMS VA'!AX32</f>
-        <v>ISIC 17T18</v>
-      </c>
-      <c r="K11" t="str">
-        <f>'KLEMS VA'!AY32</f>
-        <v>ISIC 19</v>
-      </c>
-      <c r="L11" t="str">
-        <f>'KLEMS VA'!AZ32</f>
-        <v>ISIC 20</v>
-      </c>
-      <c r="M11" t="str">
-        <f>'KLEMS VA'!BA32</f>
-        <v>ISIC 21</v>
-      </c>
-      <c r="N11" t="str">
-        <f>'KLEMS VA'!BB32</f>
-        <v>ISIC 22</v>
-      </c>
-      <c r="O11" t="str">
-        <f>'KLEMS VA'!BC32</f>
-        <v>ISIC 23</v>
-      </c>
-      <c r="P11" t="str">
-        <f>'KLEMS VA'!BD32</f>
-        <v>ISIC 24</v>
-      </c>
-      <c r="Q11" t="str">
-        <f>'KLEMS VA'!BE32</f>
-        <v>ISIC 25</v>
-      </c>
-      <c r="R11" t="str">
-        <f>'KLEMS VA'!BF32</f>
-        <v>ISIC 26</v>
-      </c>
-      <c r="S11" t="str">
-        <f>'KLEMS VA'!BG32</f>
-        <v>ISIC 27</v>
-      </c>
-      <c r="T11" t="str">
-        <f>'KLEMS VA'!BH32</f>
-        <v>ISIC 28</v>
-      </c>
-      <c r="U11" t="str">
-        <f>'KLEMS VA'!BI32</f>
-        <v>ISIC 29</v>
-      </c>
-      <c r="V11" t="str">
-        <f>'KLEMS VA'!BJ32</f>
-        <v>ISIC 30</v>
-      </c>
-      <c r="W11" t="str">
-        <f>'KLEMS VA'!BK32</f>
-        <v>ISIC 31T33</v>
-      </c>
-      <c r="X11" t="str">
-        <f>'KLEMS VA'!BL32</f>
-        <v>ISIC 35T39</v>
-      </c>
-      <c r="Y11" t="str">
-        <f>'KLEMS VA'!BM32</f>
-        <v>ISIC 41T43</v>
-      </c>
-      <c r="Z11" t="str">
-        <f>'KLEMS VA'!BN32</f>
-        <v>ISIC 45T47</v>
-      </c>
-      <c r="AA11" t="str">
-        <f>'KLEMS VA'!BO32</f>
-        <v>ISIC 49T53</v>
-      </c>
-      <c r="AB11" t="str">
-        <f>'KLEMS VA'!BP32</f>
-        <v>ISIC 55T56</v>
-      </c>
-      <c r="AC11" t="str">
-        <f>'KLEMS VA'!BQ32</f>
-        <v>ISIC 58T60</v>
-      </c>
-      <c r="AD11" t="str">
-        <f>'KLEMS VA'!BR32</f>
-        <v>ISIC 61</v>
-      </c>
-      <c r="AE11" t="str">
-        <f>'KLEMS VA'!BS32</f>
-        <v>ISIC 62T63</v>
-      </c>
-      <c r="AF11" t="str">
-        <f>'KLEMS VA'!BT32</f>
-        <v>ISIC 64T66</v>
-      </c>
-      <c r="AG11" t="str">
-        <f>'KLEMS VA'!BU32</f>
-        <v>ISIC 68</v>
-      </c>
-      <c r="AH11" t="str">
-        <f>'KLEMS VA'!BV32</f>
-        <v>ISIC 69T82</v>
-      </c>
-      <c r="AI11" t="str">
-        <f>'KLEMS VA'!BW32</f>
-        <v>ISIC 84</v>
-      </c>
-      <c r="AJ11" t="str">
-        <f>'KLEMS VA'!BX32</f>
-        <v>ISIC 85</v>
-      </c>
-      <c r="AK11" t="str">
-        <f>'KLEMS VA'!BY32</f>
-        <v>ISIC 86T88</v>
-      </c>
-      <c r="AL11" t="str">
-        <f>'KLEMS VA'!BZ32</f>
-        <v>ISIC 90T96</v>
-      </c>
-      <c r="AM11" t="str">
-        <f>'KLEMS VA'!CA32</f>
-        <v>ISIC 97T98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B12">
-        <f>B5*$B$8</f>
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:AM12" si="0">C5*$B$8</f>
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>809.06663948648361</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>2717.6518404387966</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>10376.980446158565</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>15986.100816618698</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>2069.1719110315107</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
-        <v>3222.2632868897022</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="0"/>
-        <v>17016.22398781835</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="0"/>
-        <v>2927.6650660439054</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="0"/>
-        <v>1907.7638366012293</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="0"/>
-        <v>7918.4494614717541</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>9616.7328277701145</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="0"/>
-        <v>9842.7089862732828</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="0"/>
-        <v>3445.8666940703656</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="0"/>
-        <v>4377.8462595858964</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="0"/>
-        <v>8712.7082522337969</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="0"/>
-        <v>15049.236086182249</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="0"/>
-        <v>7492.2074425811879</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="0"/>
-        <v>4053.4600451066767</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <f t="shared" si="0"/>
-        <v>59798.02715513447</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="0"/>
-        <v>86578.438587076875</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="0"/>
-        <v>35762.212828859716</v>
-      </c>
-      <c r="AB12">
-        <f t="shared" si="0"/>
-        <v>8004.8262706878268</v>
-      </c>
-      <c r="AC12">
-        <f t="shared" si="0"/>
-        <v>3865.0914976252993</v>
-      </c>
-      <c r="AD12">
-        <f t="shared" si="0"/>
-        <v>13283.091185465284</v>
-      </c>
-      <c r="AE12">
-        <f t="shared" si="0"/>
-        <v>20543.061725852112</v>
-      </c>
-      <c r="AF12">
-        <f t="shared" si="0"/>
-        <v>63484.819175410121</v>
-      </c>
-      <c r="AG12">
-        <f t="shared" si="0"/>
-        <v>55494.165596838357</v>
-      </c>
-      <c r="AH12">
-        <f t="shared" si="0"/>
-        <v>92846.727890863258</v>
-      </c>
-      <c r="AI12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AK12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AL12">
-        <f t="shared" si="0"/>
-        <v>14356.734199824075</v>
-      </c>
-      <c r="AM12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>204</v>
-      </c>
-      <c r="B13" s="27">
-        <f>B12/'KLEMS VA'!AP33</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="27">
-        <f>C12/'KLEMS VA'!AQ33</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="27">
-        <f>D12/'KLEMS VA'!AR33</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="27">
-        <f>E12/'KLEMS VA'!AS33</f>
-        <v>1.8458979668158664E-2</v>
-      </c>
-      <c r="F13" s="27">
-        <f>F12/'KLEMS VA'!AT33</f>
-        <v>4.4301551203580786E-2</v>
-      </c>
-      <c r="G13" s="27">
-        <f>G12/'KLEMS VA'!AU33</f>
-        <v>3.1380265435869727E-2</v>
-      </c>
-      <c r="H13" s="27">
-        <f>H12/'KLEMS VA'!AV33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="I13" s="27">
-        <f>I12/'KLEMS VA'!AW33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="J13" s="27">
-        <f>J12/'KLEMS VA'!AX33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="K13" s="27">
-        <f>K12/'KLEMS VA'!AY33</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="27">
-        <f>L12/'KLEMS VA'!AZ33</f>
-        <v>6.6452326805371192E-2</v>
-      </c>
-      <c r="M13" s="27">
-        <f>M12/'KLEMS VA'!BA33</f>
-        <v>1.8458979668158664E-2</v>
-      </c>
-      <c r="N13" s="27">
-        <f>N12/'KLEMS VA'!BB33</f>
-        <v>1.8458979668158661E-2</v>
-      </c>
-      <c r="O13" s="27">
-        <f>O12/'KLEMS VA'!BC33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="P13" s="27">
-        <f>P12/'KLEMS VA'!BD33</f>
-        <v>4.4301551203580786E-2</v>
-      </c>
-      <c r="Q13" s="27">
-        <f>Q12/'KLEMS VA'!BE33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="R13" s="27">
-        <f>R12/'KLEMS VA'!BF33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="S13" s="27">
-        <f>S12/'KLEMS VA'!BG33</f>
-        <v>4.4301551203580786E-2</v>
-      </c>
-      <c r="T13" s="27">
-        <f>T12/'KLEMS VA'!BH33</f>
-        <v>4.4301551203580786E-2</v>
-      </c>
-      <c r="U13" s="27">
-        <f>U12/'KLEMS VA'!BI33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="V13" s="27">
-        <f>V12/'KLEMS VA'!BJ33</f>
-        <v>6.6452326805371192E-2</v>
-      </c>
-      <c r="W13" s="27">
-        <f>W12/'KLEMS VA'!BK33</f>
-        <v>4.4301551203580786E-2</v>
-      </c>
-      <c r="X13" s="27">
-        <f>X12/'KLEMS VA'!BL33</f>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="27">
-        <f>Y12/'KLEMS VA'!BM33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="Z13" s="27">
-        <f>Z12/'KLEMS VA'!BN33</f>
-        <v>4.4301551203580786E-2</v>
-      </c>
-      <c r="AA13" s="27">
-        <f>AA12/'KLEMS VA'!BO33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="AB13" s="27">
-        <f>AB12/'KLEMS VA'!BP33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="AC13" s="27">
-        <f>AC12/'KLEMS VA'!BQ33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="AD13" s="27">
-        <f>AD12/'KLEMS VA'!BR33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="AE13" s="27">
-        <f>AE12/'KLEMS VA'!BS33</f>
-        <v>4.4301551203580793E-2</v>
-      </c>
-      <c r="AF13" s="27">
-        <f>AF12/'KLEMS VA'!BT33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="AG13" s="27">
-        <f>AG12/'KLEMS VA'!BU33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="AH13" s="27">
-        <f>AH12/'KLEMS VA'!BV33</f>
-        <v>6.6452326805371179E-2</v>
-      </c>
-      <c r="AI13" s="27">
-        <f>AI12/'KLEMS VA'!BW33</f>
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="27">
-        <f>AJ12/'KLEMS VA'!BX33</f>
-        <v>0</v>
-      </c>
-      <c r="AK13" s="27">
-        <f>AK12/'KLEMS VA'!BY33</f>
-        <v>0</v>
-      </c>
-      <c r="AL13" s="27">
-        <f>AL12/'KLEMS VA'!BZ33</f>
-        <v>6.6452326805371192E-2</v>
-      </c>
-      <c r="AM13" s="27">
-        <f>AM12/'KLEMS VA'!CA33</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -9129,155 +7598,155 @@
         <v>40</v>
       </c>
       <c r="B2" s="9">
-        <f>'Corporate Taxes'!B4+GST!B13</f>
+        <f>'Corporate Taxes'!B4</f>
         <v>4.551107569199989E-4</v>
       </c>
       <c r="C2" s="9">
-        <f>'Corporate Taxes'!C4+GST!C13</f>
+        <f>'Corporate Taxes'!C4</f>
         <v>5.593526565219218E-2</v>
       </c>
       <c r="D2" s="9">
-        <f>'Corporate Taxes'!D4+GST!D13</f>
+        <f>'Corporate Taxes'!D4</f>
         <v>0.1262807486599779</v>
       </c>
       <c r="E2" s="9">
-        <f>'Corporate Taxes'!E4+GST!E13</f>
-        <v>0.17811623057471859</v>
+        <f>'Corporate Taxes'!E4</f>
+        <v>0.15965725090655994</v>
       </c>
       <c r="F2" s="9">
-        <f>'Corporate Taxes'!F4+GST!F13</f>
-        <v>4.4301551203580786E-2</v>
+        <f>'Corporate Taxes'!F4</f>
+        <v>0</v>
       </c>
       <c r="G2" s="9">
-        <f>'Corporate Taxes'!G4+GST!G13</f>
-        <v>6.0050578278672301E-2</v>
+        <f>'Corporate Taxes'!G4</f>
+        <v>2.8670312842802578E-2</v>
       </c>
       <c r="H2" s="9">
-        <f>'Corporate Taxes'!H4+GST!H13</f>
-        <v>5.6161466684957723E-2</v>
+        <f>'Corporate Taxes'!H4</f>
+        <v>1.1859915481376927E-2</v>
       </c>
       <c r="I2" s="9">
-        <f>'Corporate Taxes'!I4+GST!I13</f>
-        <v>0.16770563361314783</v>
+        <f>'Corporate Taxes'!I4</f>
+        <v>0.12340408240956703</v>
       </c>
       <c r="J2" s="9">
-        <f>'Corporate Taxes'!J4+GST!J13</f>
-        <v>6.7686514421438998E-2</v>
+        <f>'Corporate Taxes'!J4</f>
+        <v>2.3384963217858205E-2</v>
       </c>
       <c r="K2" s="9">
-        <f>'Corporate Taxes'!K4+GST!K13</f>
+        <f>'Corporate Taxes'!K4</f>
         <v>0.1397347927906448</v>
       </c>
       <c r="L2" s="9">
-        <f>'Corporate Taxes'!L4+GST!L13</f>
-        <v>0.11399046000801358</v>
+        <f>'Corporate Taxes'!L4</f>
+        <v>4.7538133202642378E-2</v>
       </c>
       <c r="M2" s="9">
-        <f>'Corporate Taxes'!M4+GST!M13</f>
-        <v>0.12091274090452887</v>
+        <f>'Corporate Taxes'!M4</f>
+        <v>0.10245376123637021</v>
       </c>
       <c r="N2" s="9">
-        <f>'Corporate Taxes'!N4+GST!N13</f>
-        <v>5.0951095843226497E-2</v>
+        <f>'Corporate Taxes'!N4</f>
+        <v>3.2492116175067837E-2</v>
       </c>
       <c r="O2" s="9">
-        <f>'Corporate Taxes'!O4+GST!O13</f>
-        <v>6.3921246517373437E-2</v>
+        <f>'Corporate Taxes'!O4</f>
+        <v>1.9619695313792637E-2</v>
       </c>
       <c r="P2" s="9">
-        <f>'Corporate Taxes'!P4+GST!P13</f>
-        <v>9.7379987826788972E-2</v>
+        <f>'Corporate Taxes'!P4</f>
+        <v>5.3078436623208186E-2</v>
       </c>
       <c r="Q2" s="9">
-        <f>'Corporate Taxes'!Q4+GST!Q13</f>
-        <v>0.18985640921493821</v>
+        <f>'Corporate Taxes'!Q4</f>
+        <v>0.12340408240956703</v>
       </c>
       <c r="R2" s="9">
-        <f>'Corporate Taxes'!R4+GST!R13</f>
-        <v>9.9354636419035178E-2</v>
+        <f>'Corporate Taxes'!R4</f>
+        <v>3.2902309613663999E-2</v>
       </c>
       <c r="S2" s="9">
-        <f>'Corporate Taxes'!S4+GST!S13</f>
-        <v>0.16770563361314783</v>
+        <f>'Corporate Taxes'!S4</f>
+        <v>0.12340408240956703</v>
       </c>
       <c r="T2" s="9">
-        <f>'Corporate Taxes'!T4+GST!T13</f>
-        <v>0.16770563361314783</v>
+        <f>'Corporate Taxes'!T4</f>
+        <v>0.12340408240956703</v>
       </c>
       <c r="U2" s="9">
-        <f>'Corporate Taxes'!U4+GST!U13</f>
-        <v>9.9622590799401223E-2</v>
+        <f>'Corporate Taxes'!U4</f>
+        <v>3.3170263994030037E-2</v>
       </c>
       <c r="V2" s="9">
-        <f>'Corporate Taxes'!V4+GST!V13</f>
-        <v>9.9622590799401223E-2</v>
+        <f>'Corporate Taxes'!V4</f>
+        <v>3.3170263994030037E-2</v>
       </c>
       <c r="W2" s="9">
-        <f>'Corporate Taxes'!W4+GST!W13</f>
-        <v>0.16770563361314783</v>
+        <f>'Corporate Taxes'!W4</f>
+        <v>0.12340408240956703</v>
       </c>
       <c r="X2" s="9">
-        <f>'Corporate Taxes'!X4+GST!X13</f>
+        <f>'Corporate Taxes'!X4</f>
         <v>3.8379514776179789E-4</v>
       </c>
       <c r="Y2" s="9">
-        <f>'Corporate Taxes'!Y4+GST!Y13</f>
-        <v>5.6802187085498772E-2</v>
+        <f>'Corporate Taxes'!Y4</f>
+        <v>1.2500635881917981E-2</v>
       </c>
       <c r="Z2" s="9">
-        <f>'Corporate Taxes'!Z4+GST!Z13</f>
-        <v>5.7260259824567249E-2</v>
+        <f>'Corporate Taxes'!Z4</f>
+        <v>1.2958708620986461E-2</v>
       </c>
       <c r="AA2" s="9">
-        <f>'Corporate Taxes'!AA4+GST!AA13</f>
-        <v>5.0943882752661901E-2</v>
+        <f>'Corporate Taxes'!AA4</f>
+        <v>6.6423315490811118E-3</v>
       </c>
       <c r="AB2" s="9">
-        <f>'Corporate Taxes'!AB4+GST!AB13</f>
-        <v>5.4955129453449936E-2</v>
+        <f>'Corporate Taxes'!AB4</f>
+        <v>1.0653578249869147E-2</v>
       </c>
       <c r="AC2" s="9">
-        <f>'Corporate Taxes'!AC4+GST!AC13</f>
-        <v>6.6452326805371179E-2</v>
+        <f>'Corporate Taxes'!AC4</f>
+        <v>0</v>
       </c>
       <c r="AD2" s="9">
-        <f>'Corporate Taxes'!AD4+GST!AD13</f>
-        <v>9.7507957930944675E-2</v>
+        <f>'Corporate Taxes'!AD4</f>
+        <v>3.1055631125573493E-2</v>
       </c>
       <c r="AE2" s="9">
-        <f>'Corporate Taxes'!AE4+GST!AE13</f>
-        <v>0.16172989661622766</v>
+        <f>'Corporate Taxes'!AE4</f>
+        <v>0.11742834541264688</v>
       </c>
       <c r="AF2" s="9">
-        <f>'Corporate Taxes'!AF4+GST!AF13</f>
-        <v>0.17697466308416615</v>
+        <f>'Corporate Taxes'!AF4</f>
+        <v>0.11052233627879497</v>
       </c>
       <c r="AG2" s="9">
-        <f>'Corporate Taxes'!AG4+GST!AG13</f>
-        <v>7.4453980228034358E-2</v>
+        <f>'Corporate Taxes'!AG4</f>
+        <v>8.0016534226631832E-3</v>
       </c>
       <c r="AH2" s="9">
-        <f>'Corporate Taxes'!AH4+GST!AH13</f>
-        <v>9.2265918203077807E-2</v>
+        <f>'Corporate Taxes'!AH4</f>
+        <v>2.5813591397706628E-2</v>
       </c>
       <c r="AI2" s="9">
-        <f>'Corporate Taxes'!AI4+GST!AI13</f>
+        <f>'Corporate Taxes'!AI4</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="9">
-        <f>'Corporate Taxes'!AJ4+GST!AJ13</f>
+        <f>'Corporate Taxes'!AJ4</f>
         <v>1.0408780643824105E-3</v>
       </c>
       <c r="AK2" s="9">
-        <f>'Corporate Taxes'!AK4+GST!AK13</f>
+        <f>'Corporate Taxes'!AK4</f>
         <v>8.1104834345487389E-3</v>
       </c>
       <c r="AL2" s="9">
-        <f>'Corporate Taxes'!AL4+GST!AL13</f>
-        <v>8.3309183177282475E-2</v>
+        <f>'Corporate Taxes'!AL4</f>
+        <v>1.6856856371911283E-2</v>
       </c>
       <c r="AM2" s="9">
-        <f>'Corporate Taxes'!AM4+GST!AM13</f>
+        <f>'Corporate Taxes'!AM4</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>